<commit_message>
feat: Ankara hastaneleri eklendi (67 hastane)
Toplam: 1651 hastane, 82 il
- Ankara Kamu/Üniversite: 58 hastane
- Ankara Özel: 9 hastane
</commit_message>
<xml_diff>
--- a/Hastane listesi tam.xlsx
+++ b/Hastane listesi tam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\HEALMEDY\ABROV2\lockdownsofthbys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFF7377D-BA41-43F1-8BEB-4AA10FE30349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ED31DD-BDE9-469E-B481-9E382D916A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3B60585D-3D33-409D-B429-66580BD557D1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6059" uniqueCount="1740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6260" uniqueCount="1807">
   <si>
     <t>İl</t>
   </si>
@@ -5257,6 +5257,207 @@
   </si>
   <si>
     <t>Özel Başarı Hastanesi, Gaziosmanpaşa</t>
+  </si>
+  <si>
+    <t>Ankara Bilkent Şehir Hastanesi</t>
+  </si>
+  <si>
+    <t>Ankara Etlik Şehir Hastanesi</t>
+  </si>
+  <si>
+    <t>Ankara Atatürk Sanatoryum Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Ankara Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Gülhane Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Dışkapı Yıldırım Beyazıt Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Dr. Abdurrahman Yurtaslan Ankara Onkoloji Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Etlik Zübeyde Hanım Kadın Hastalıkları Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Sincan Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Ankara Dr. Sami Ulus Çocuk Sağlığı ve Hastalıkları Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Ankara Gaziler Fizik Tedavi ve Rehabilitasyon Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Ulucanlar Göz Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>Yenimahalle Eğitim ve Araştırma Hastanesi</t>
+  </si>
+  <si>
+    <t>75. Yıl Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Osmanlı Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Polatlı Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Balgat Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Etimesgut Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Ülkü Ulusoy Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Karapürçek Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Mamak Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Pursaklar Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Sincan Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Tepebaşı Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Topraklık Ağız ve Diş Sağlığı Hastanesi</t>
+  </si>
+  <si>
+    <t>Ankara Beştepe Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Akyurt Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Ayaş Şehit Mehmet Çifci Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Bala Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Beştepe Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Beypazarı Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Beytepe Şehit Murat Erdi Eker Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Ceza İnfaz Kurumları Kampüs Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Çubuk Halil Şıvgın Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Elmadağ Dr. Hulusi Alataş Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Etimesgut Şehit Sait Ertürk Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Gazi Mustafa Kemal Mesleki ve Çevresel Hastalıklar Hastanesi</t>
+  </si>
+  <si>
+    <t>Gölbaşı Şehit Ahmet Özsoy Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Güdül İlçe Entegre Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Haymana Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Kahramankazan Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Kalecik İlçe Entegre Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Kızılcahamam Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Mamak Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Nallıhan Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Polatlı Duatepe Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Pursaklar Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Şereflikoçhisar Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>29 Mayıs Devlet Hastanesi</t>
+  </si>
+  <si>
+    <t>Ankara Üniversitesi Cebeci Araştırma ve Uygulama Hastanesi</t>
+  </si>
+  <si>
+    <t>Ankara Üniversitesi İbni Sina Araştırma ve Uygulama Hastanesi</t>
+  </si>
+  <si>
+    <t>Başkent Üniversitesi Ankara Hastanesi</t>
+  </si>
+  <si>
+    <t>Gazi Üniversitesi Tıp Fakültesi Hastanesi</t>
+  </si>
+  <si>
+    <t>Hacettepe Üniversitesi Beytepe Gün Hastanesi</t>
+  </si>
+  <si>
+    <t>Hacettepe Üniversitesi Erişkin Hastanesi</t>
+  </si>
+  <si>
+    <t>Hacettepe Üniversitesi İhsan Doğramacı Çocuk Hastanesi</t>
+  </si>
+  <si>
+    <t>Hacettepe Üniversitesi Onkoloji Hastanesi</t>
+  </si>
+  <si>
+    <t>Ufuk Üniversitesi Dr. Rıdvan Ege Hastanesi</t>
+  </si>
+  <si>
+    <t>Bayındır Hastanesi</t>
+  </si>
+  <si>
+    <t>Dünya Göz Hastanesi (Çankaya)</t>
+  </si>
+  <si>
+    <t>Dünya Göz Hastanesi Keçiören</t>
+  </si>
+  <si>
+    <t>Dünya Göz Hastanesi Sincan</t>
+  </si>
+  <si>
+    <t>Güven Hastanesi</t>
+  </si>
+  <si>
+    <t>Medical Park (Yenimahalle)</t>
+  </si>
+  <si>
+    <t>Medical Park Keçiören</t>
+  </si>
+  <si>
+    <t>Mega Avrupa Diş Hastanesi</t>
+  </si>
+  <si>
+    <t>TOBB ETÜ Hastanesi</t>
   </si>
 </sst>
 </file>
@@ -5629,10 +5830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6A4D8-D155-4044-BA73-0D68C59E42EB}">
-  <dimension ref="A1:C1579"/>
+  <dimension ref="A1:C1652"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1405" workbookViewId="0">
-      <selection activeCell="E1417" sqref="E1417"/>
+    <sheetView tabSelected="1" topLeftCell="A1564" workbookViewId="0">
+      <selection activeCell="A1581" sqref="A1581:C1652"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22051,6 +22252,743 @@
       </c>
       <c r="C1579" t="s">
         <v>1739</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1581" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1581" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1581" t="s">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1582" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1582" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1582" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1584" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1584" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1584" t="s">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1585" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1585" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1585" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1586" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1586" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1586" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1587" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1587" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1587" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1588" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1588" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1588" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1589" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1589" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1589" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1590" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1590" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1590" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1591" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1591" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1591" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1592" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1592" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1592" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1593" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1593" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1593" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1594" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1594" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1594" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1596" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1596" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1596" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1597" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1597" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1597" t="s">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1598" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1598" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1598" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1599" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1599" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1599" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1600" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1600" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1600" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1601" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1601" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1601" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1602" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1602" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1602" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1603" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1603" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1603" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1604" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1604" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1604" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1605" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1605" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1605" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1606" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1606" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1606" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1607" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1607" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1607" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1609" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1609" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1609" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1610" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1610" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1610" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1611" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1611" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1611" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1612" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1612" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1612" t="s">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1613" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1613" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1613" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1614" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1614" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1614" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1615" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1615" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1615" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1616" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1616" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1616" t="s">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1617" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1617" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1617" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1618" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1618" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1618" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1619" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1619" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1619" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1620" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1620" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1620" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1621" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1621" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1621" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1622" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1622" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1622" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1623" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1623" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1623" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1624" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1624" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1624" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1625" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1625" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1625" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1626" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1626" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1626" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1627" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1627" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1627" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1628" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1628" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1628" t="s">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1629" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1629" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1629" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1630" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1630" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1630" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1631" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1631" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1631" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1632" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1632" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1632" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1634" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1634" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1634" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1635" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1635" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1635" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1636" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1636" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1636" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1637" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1637" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1637" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1638" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1638" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1638" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1639" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1639" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1639" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1640" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1640" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1640" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1641" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1641" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1641" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1642" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1642" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1642" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1644" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1644" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1644" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1645" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1645" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1645" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1646" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1646" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1646" t="s">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1647" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1647" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1647" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1648" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1648" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1648" t="s">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1649" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1649" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1649" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1650" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1650" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1650" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1651" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1651" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1651" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1652" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1652" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1652" t="s">
+        <v>1806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: PDF editor icin hazir kutucuklar eklendi, ornek PDF sablonu olusturuldu
</commit_message>
<xml_diff>
--- a/Hastane listesi tam.xlsx
+++ b/Hastane listesi tam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\HEALMEDY\ABROV2\lockdownsofthbys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ED31DD-BDE9-469E-B481-9E382D916A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55ED197-AB7D-4451-8F95-9C18D1925A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3B60585D-3D33-409D-B429-66580BD557D1}"/>
   </bookViews>
@@ -5832,8 +5832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6A4D8-D155-4044-BA73-0D68C59E42EB}">
   <dimension ref="A1:C1652"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1564" workbookViewId="0">
-      <selection activeCell="A1581" sqref="A1581:C1652"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="C234" sqref="C234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>